<commit_message>
Added MOSFET models, updated info
</commit_message>
<xml_diff>
--- a/DOCS/Part list.xlsx
+++ b/DOCS/Part list.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763B93E0-7DAE-4A3D-8F4C-6883C8C0A403}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056C401D-3816-4EDA-92B2-564BBAABBDB4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Part</t>
   </si>
@@ -55,9 +55,6 @@
     <t>LTC1865</t>
   </si>
   <si>
-    <t>Current Op Amp</t>
-  </si>
-  <si>
     <t>LT1014</t>
   </si>
   <si>
@@ -70,10 +67,88 @@
     <t>Total</t>
   </si>
   <si>
-    <t>12-bit 2ch DAC</t>
-  </si>
-  <si>
     <t>610 3-2-5</t>
+  </si>
+  <si>
+    <t>12-bit 2ch ADC</t>
+  </si>
+  <si>
+    <t>Bypass MOSFET</t>
+  </si>
+  <si>
+    <t>SIRC10DP</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Op amp</t>
+  </si>
+  <si>
+    <t>Sense resistor</t>
+  </si>
+  <si>
+    <t>0R002</t>
+  </si>
+  <si>
+    <t>2R</t>
+  </si>
+  <si>
+    <t>Trimmer pot</t>
+  </si>
+  <si>
+    <t>6+</t>
+  </si>
+  <si>
+    <t>2+</t>
+  </si>
+  <si>
+    <t>Temp sensor</t>
+  </si>
+  <si>
+    <t>Isolator</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>DPDT switch</t>
+  </si>
+  <si>
+    <t>20k, SMD</t>
+  </si>
+  <si>
+    <t>LM50C</t>
+  </si>
+  <si>
+    <t>610 3-14-1</t>
+  </si>
+  <si>
+    <t>+5V Linear reg.</t>
+  </si>
+  <si>
+    <t>-5V Linear reg.</t>
+  </si>
+  <si>
+    <t>78L05</t>
+  </si>
+  <si>
+    <t>79L05</t>
+  </si>
+  <si>
+    <t>+12V Linear reg</t>
+  </si>
+  <si>
+    <t>78L12</t>
+  </si>
+  <si>
+    <t>OPA349?</t>
+  </si>
+  <si>
+    <t>MAX743</t>
+  </si>
+  <si>
+    <t>+5V to +-15V, +-12V</t>
   </si>
 </sst>
 </file>
@@ -428,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -440,7 +515,7 @@
     <col min="3" max="16384" width="9.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -457,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -489,67 +564,256 @@
         <v>31.363200000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1">
+        <v>524</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1">
+        <v>524</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1">
+        <v>524</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1">
+        <v>524</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1">
+        <v>524</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{C28776B6-4996-4B8B-B4C0-689033314BD1}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{1481F52E-3B69-4F62-9C35-4F6D3275EFD2}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{4D6F4ECD-DBFA-4624-A3AF-0794612D62D7}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{95D79344-594B-4A90-AE58-2C551EC6EDF4}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{B78BF082-5284-4E31-8179-AEE6DF78E252}"/>
+    <hyperlink ref="B13" r:id="rId3" xr:uid="{4D6F4ECD-DBFA-4624-A3AF-0794612D62D7}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{95D79344-594B-4A90-AE58-2C551EC6EDF4}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{B78BF082-5284-4E31-8179-AEE6DF78E252}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed measurement opamps to OPA77
</commit_message>
<xml_diff>
--- a/DOCS/Part list.xlsx
+++ b/DOCS/Part list.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056C401D-3816-4EDA-92B2-564BBAABBDB4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4936D50B-3687-4AF6-B6C3-CE9FF98D3869}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Used" sheetId="1" r:id="rId1"/>
+    <sheet name="Available" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="141">
   <si>
     <t>Part</t>
   </si>
@@ -88,9 +89,6 @@
     <t>Sense resistor</t>
   </si>
   <si>
-    <t>0R002</t>
-  </si>
-  <si>
     <t>2R</t>
   </si>
   <si>
@@ -149,6 +147,303 @@
   </si>
   <si>
     <t>+5V to +-15V, +-12V</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>OpAmp</t>
+  </si>
+  <si>
+    <t>Vol.reg.</t>
+  </si>
+  <si>
+    <t>Temp.</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Opto</t>
+  </si>
+  <si>
+    <t>4N37</t>
+  </si>
+  <si>
+    <t>610-IC</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>AD1582</t>
+  </si>
+  <si>
+    <t>AD620</t>
+  </si>
+  <si>
+    <t>AD677</t>
+  </si>
+  <si>
+    <t>AD707</t>
+  </si>
+  <si>
+    <t>AD8065</t>
+  </si>
+  <si>
+    <t>AD9235</t>
+  </si>
+  <si>
+    <t>DAC08</t>
+  </si>
+  <si>
+    <t>EL2044CSZ</t>
+  </si>
+  <si>
+    <t>FOD817A</t>
+  </si>
+  <si>
+    <t>HCNW2611</t>
+  </si>
+  <si>
+    <t>HCPL-061N</t>
+  </si>
+  <si>
+    <t>HCPL-063N</t>
+  </si>
+  <si>
+    <t>LC549</t>
+  </si>
+  <si>
+    <t>LF412C</t>
+  </si>
+  <si>
+    <t>LM20</t>
+  </si>
+  <si>
+    <t>LM2573</t>
+  </si>
+  <si>
+    <t>LM2671</t>
+  </si>
+  <si>
+    <t>LM2674</t>
+  </si>
+  <si>
+    <t>LM317L</t>
+  </si>
+  <si>
+    <t>LM50</t>
+  </si>
+  <si>
+    <t>LM5576</t>
+  </si>
+  <si>
+    <t>LM7121</t>
+  </si>
+  <si>
+    <t>LM75A</t>
+  </si>
+  <si>
+    <t>LM837</t>
+  </si>
+  <si>
+    <t>LMC660</t>
+  </si>
+  <si>
+    <t>LMC662</t>
+  </si>
+  <si>
+    <t>LP2985AIM5-3.0</t>
+  </si>
+  <si>
+    <t>LP2985AIM5-3.1</t>
+  </si>
+  <si>
+    <t>LT1761</t>
+  </si>
+  <si>
+    <t>LT1964</t>
+  </si>
+  <si>
+    <t>LTC1261</t>
+  </si>
+  <si>
+    <t>LTC1453</t>
+  </si>
+  <si>
+    <t>M109A</t>
+  </si>
+  <si>
+    <t>MAX518</t>
+  </si>
+  <si>
+    <t>PC355</t>
+  </si>
+  <si>
+    <t>PCF8591</t>
+  </si>
+  <si>
+    <t>SFH6156</t>
+  </si>
+  <si>
+    <t>TL051C</t>
+  </si>
+  <si>
+    <t>TL317</t>
+  </si>
+  <si>
+    <t>TLC27L4B</t>
+  </si>
+  <si>
+    <t>TPS40055-EP</t>
+  </si>
+  <si>
+    <t>TPS767D301</t>
+  </si>
+  <si>
+    <t>XC6209F312MR</t>
+  </si>
+  <si>
+    <t>UA748CDP</t>
+  </si>
+  <si>
+    <t>LM837N</t>
+  </si>
+  <si>
+    <t>LM358N</t>
+  </si>
+  <si>
+    <t>LF412CN</t>
+  </si>
+  <si>
+    <t>LF357</t>
+  </si>
+  <si>
+    <t>ICL7660CPA</t>
+  </si>
+  <si>
+    <t>ICL7612BCPA</t>
+  </si>
+  <si>
+    <t>GL358</t>
+  </si>
+  <si>
+    <t>AMP01FX</t>
+  </si>
+  <si>
+    <t>610-DIP</t>
+  </si>
+  <si>
+    <t>27L2C</t>
+  </si>
+  <si>
+    <t>27L4AC</t>
+  </si>
+  <si>
+    <t>TS9241</t>
+  </si>
+  <si>
+    <t>TS902ID</t>
+  </si>
+  <si>
+    <t>TPS54616</t>
+  </si>
+  <si>
+    <t>TLC274CD</t>
+  </si>
+  <si>
+    <t>TLC271</t>
+  </si>
+  <si>
+    <t>TLC074CN</t>
+  </si>
+  <si>
+    <t>TL084</t>
+  </si>
+  <si>
+    <t>TL082CP</t>
+  </si>
+  <si>
+    <t>TL074</t>
+  </si>
+  <si>
+    <t>TL064CD</t>
+  </si>
+  <si>
+    <t>TCA0372</t>
+  </si>
+  <si>
+    <t>S-81250AG</t>
+  </si>
+  <si>
+    <t>OPA77FP</t>
+  </si>
+  <si>
+    <t>OPA349</t>
+  </si>
+  <si>
+    <t>OPA2137</t>
+  </si>
+  <si>
+    <t>OP77E</t>
+  </si>
+  <si>
+    <t>LTC1663CS5</t>
+  </si>
+  <si>
+    <t>LT1004CZ12</t>
+  </si>
+  <si>
+    <t>LS204CN</t>
+  </si>
+  <si>
+    <t>LMC662AIN</t>
+  </si>
+  <si>
+    <t>LM79L05ACM</t>
+  </si>
+  <si>
+    <t>LM45BIM3</t>
+  </si>
+  <si>
+    <t>LM35D</t>
+  </si>
+  <si>
+    <t>LM258</t>
+  </si>
+  <si>
+    <t>LM2576HVT-ADJ</t>
+  </si>
+  <si>
+    <t>LM1089CS-ADJ</t>
+  </si>
+  <si>
+    <t>LM78M05CS</t>
+  </si>
+  <si>
+    <t>L4885CV</t>
+  </si>
+  <si>
+    <t>IL223AT</t>
+  </si>
+  <si>
+    <t>DS11307</t>
+  </si>
+  <si>
+    <t>AD8532AR</t>
+  </si>
+  <si>
+    <t>AD811</t>
+  </si>
+  <si>
+    <t>524-Mikro</t>
+  </si>
+  <si>
+    <t>0R004</t>
   </si>
 </sst>
 </file>
@@ -182,12 +477,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -204,7 +505,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -219,6 +520,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -506,7 +813,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -557,11 +864,11 @@
         <v>15.681600000000001</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="5">
         <f>F2*E2</f>
-        <v>31.363200000000003</v>
+        <v>47.044800000000002</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -569,17 +876,25 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="4">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="E3" s="4">
+        <f>D3*1.21</f>
+        <v>0.74656999999999996</v>
+      </c>
       <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <f>F3*E3</f>
+        <v>2.9862799999999998</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -590,10 +905,10 @@
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C5" s="1">
         <v>524</v>
@@ -616,7 +931,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -627,10 +942,10 @@
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1">
         <v>524</v>
@@ -638,19 +953,19 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -661,7 +976,7 @@
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -683,10 +998,10 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -702,7 +1017,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -723,10 +1038,10 @@
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C14" s="1">
         <v>524</v>
@@ -739,10 +1054,10 @@
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1">
         <v>524</v>
@@ -755,10 +1070,10 @@
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="1">
         <v>524</v>
@@ -772,10 +1087,10 @@
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -814,7 +1129,753 @@
     <hyperlink ref="B13" r:id="rId3" xr:uid="{4D6F4ECD-DBFA-4624-A3AF-0794612D62D7}"/>
     <hyperlink ref="B11" r:id="rId4" xr:uid="{95D79344-594B-4A90-AE58-2C551EC6EDF4}"/>
     <hyperlink ref="B12" r:id="rId5" xr:uid="{B78BF082-5284-4E31-8179-AEE6DF78E252}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{74C76EA8-8D4D-4593-A416-D8501506A171}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F0A316-A29F-48D0-8AC3-D29C296612BB}">
+  <dimension ref="A1:N43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="14" width="14.28515625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed packages, board layout
Changed component packages and values to the ones that are available. Moved the heatsink mount back to the PCB,
</commit_message>
<xml_diff>
--- a/DOCS/Part list.xlsx
+++ b/DOCS/Part list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{422E877A-6094-49D4-9E82-9D635A74E1E7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3D0E86-6F3E-490D-A04F-372E2590F718}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Used" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="216">
   <si>
     <t>Part</t>
   </si>
@@ -658,6 +658,18 @@
   </si>
   <si>
     <t>1-16-6</t>
+  </si>
+  <si>
+    <t>A=1206</t>
+  </si>
+  <si>
+    <t>B=1210</t>
+  </si>
+  <si>
+    <t>C=2312</t>
+  </si>
+  <si>
+    <t>D=2917</t>
   </si>
 </sst>
 </file>
@@ -665,7 +677,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -716,7 +728,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
@@ -730,10 +742,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -751,19 +763,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -779,6 +782,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1065,17 +1077,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.73046875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.73046875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.73046875" style="1"/>
+    <col min="1" max="2" width="18.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1098,7 +1110,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1124,7 +1136,7 @@
         <v>31.363200000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1149,7 +1161,7 @@
         <v>2.9862799999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>146</v>
       </c>
@@ -1174,14 +1186,14 @@
         <v>3.0975999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>148</v>
       </c>
@@ -1206,18 +1218,18 @@
         <v>17.829999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="19" t="s">
         <v>141</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1238,9 +1250,9 @@
         <v>15.9236</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1259,7 +1271,7 @@
         <v>19.432599999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1276,7 +1288,7 @@
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>143</v>
       </c>
@@ -1300,13 +1312,13 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1320,7 +1332,7 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1337,7 +1349,7 @@
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1354,7 +1366,7 @@
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1365,7 +1377,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1384,7 +1396,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1400,7 +1412,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1416,7 +1428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1432,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -1448,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
@@ -1462,10 +1474,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
@@ -1479,11 +1491,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -1499,7 +1511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
   </sheetData>
@@ -1535,43 +1547,43 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.73046875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="14.265625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.73046875" style="1"/>
+    <col min="1" max="14" width="14.28515625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11" t="s">
+      <c r="L1" s="18"/>
+      <c r="M1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="11"/>
-    </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="N1" s="18"/>
+    </row>
+    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1612,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
@@ -1656,7 +1668,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1700,7 +1712,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>64</v>
       </c>
@@ -1744,7 +1756,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1782,7 +1794,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
@@ -1820,7 +1832,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>136</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
         <v>75</v>
       </c>
@@ -1872,7 +1884,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
         <v>76</v>
       </c>
@@ -1892,7 +1904,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
         <v>77</v>
       </c>
@@ -1906,7 +1918,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E12" s="7" t="s">
         <v>11</v>
       </c>
@@ -1920,7 +1932,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
         <v>89</v>
       </c>
@@ -1934,7 +1946,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
         <v>91</v>
       </c>
@@ -1948,7 +1960,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
         <v>95</v>
       </c>
@@ -1962,7 +1974,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
         <v>96</v>
       </c>
@@ -1976,7 +1988,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>97</v>
       </c>
@@ -1990,7 +2002,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>98</v>
       </c>
@@ -2004,7 +2016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>99</v>
       </c>
@@ -2018,7 +2030,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="1" t="s">
         <v>101</v>
       </c>
@@ -2032,7 +2044,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
         <v>102</v>
       </c>
@@ -2046,7 +2058,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E22" s="1" t="s">
         <v>103</v>
       </c>
@@ -2060,7 +2072,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E23" s="1" t="s">
         <v>107</v>
       </c>
@@ -2074,7 +2086,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E24" s="1" t="s">
         <v>108</v>
       </c>
@@ -2088,7 +2100,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E25" s="1" t="s">
         <v>110</v>
       </c>
@@ -2102,7 +2114,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" s="1" t="s">
         <v>111</v>
       </c>
@@ -2116,7 +2128,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" s="1" t="s">
         <v>112</v>
       </c>
@@ -2130,7 +2142,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="1" t="s">
         <v>113</v>
       </c>
@@ -2138,7 +2150,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="1" t="s">
         <v>114</v>
       </c>
@@ -2146,7 +2158,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E30" s="1" t="s">
         <v>115</v>
       </c>
@@ -2154,7 +2166,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E31" s="1" t="s">
         <v>116</v>
       </c>
@@ -2162,7 +2174,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="s">
         <v>117</v>
       </c>
@@ -2170,7 +2182,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="7" t="s">
         <v>119</v>
       </c>
@@ -2178,7 +2190,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="1" t="s">
         <v>120</v>
       </c>
@@ -2186,7 +2198,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="s">
         <v>121</v>
       </c>
@@ -2194,7 +2206,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36" s="1" t="s">
         <v>122</v>
       </c>
@@ -2202,7 +2214,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E37" s="1" t="s">
         <v>125</v>
       </c>
@@ -2210,7 +2222,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="1" t="s">
         <v>126</v>
       </c>
@@ -2218,7 +2230,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E39" s="1" t="s">
         <v>130</v>
       </c>
@@ -2226,7 +2238,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E40" s="1" t="s">
         <v>137</v>
       </c>
@@ -2234,7 +2246,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E41" s="1" t="s">
         <v>138</v>
       </c>
@@ -2242,7 +2254,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E42" s="1" t="s">
         <v>106</v>
       </c>
@@ -2250,7 +2262,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E43" s="1" t="s">
         <v>105</v>
       </c>
@@ -2274,347 +2286,359 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D077170-5C74-45B1-BD2D-CC2883FCAE3A}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.59765625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.59765625" style="10"/>
-    <col min="2" max="2" width="9.59765625" style="13"/>
-    <col min="3" max="3" width="9.59765625" style="14"/>
-    <col min="4" max="5" width="9.59765625" style="10"/>
-    <col min="6" max="7" width="9.59765625" style="14"/>
-    <col min="8" max="8" width="18.59765625" style="14" customWidth="1"/>
-    <col min="9" max="16384" width="9.59765625" style="10"/>
+    <col min="1" max="1" width="9.5703125" style="10"/>
+    <col min="2" max="2" width="9.5703125" style="11"/>
+    <col min="3" max="3" width="9.5703125" style="12"/>
+    <col min="4" max="5" width="9.5703125" style="10"/>
+    <col min="6" max="7" width="9.5703125" style="12"/>
+    <col min="8" max="8" width="18.5703125" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="9.5703125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="11"/>
-      <c r="B2" s="13" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>154</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="13">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>156</v>
       </c>
       <c r="D3" s="10">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="12">
         <v>1206</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="12" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I3" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="13">
         <v>1E-8</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>156</v>
       </c>
       <c r="D4" s="10">
         <v>6</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="11">
         <v>1E-8</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="12" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I4" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="13">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>156</v>
       </c>
       <c r="D5" s="10">
         <v>23</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="11">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>1206</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="12" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I5" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="13">
         <v>3.3000000000000002E-7</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>156</v>
       </c>
       <c r="D6" s="10">
         <v>2</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="11">
         <v>3.3000000000000002E-7</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="12">
         <v>1206</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="12" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I6" s="10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="13">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>157</v>
       </c>
       <c r="D7" s="10">
         <v>6</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="11">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="12" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="13">
         <v>2.2000000000000001E-6</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>157</v>
       </c>
       <c r="D8" s="10">
         <v>1</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="11">
         <v>1.5E-6</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="12" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="13">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>157</v>
       </c>
       <c r="D9" s="10">
         <v>1</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="11">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="12" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="13">
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>157</v>
       </c>
       <c r="D10" s="10">
         <v>1</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="11">
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="12" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="14">
         <v>1E-4</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="15" t="s">
         <v>157</v>
       </c>
       <c r="D11" s="7">
         <v>3</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="16">
         <v>2.2000000000000001E-4</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="15" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>166</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>176</v>
       </c>
       <c r="D12" s="10">
         <v>2</v>
       </c>
-      <c r="H12" s="14">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E12" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>165</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="D13" s="10">
         <v>2</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H13" s="12">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="17">
         <v>1E-4</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="7">
         <v>2</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18">
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15">
         <v>524</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>171</v>
       </c>
       <c r="D15" s="10">
@@ -2623,21 +2647,21 @@
       <c r="E15" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="12" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>171</v>
       </c>
       <c r="D16" s="10">
@@ -2646,318 +2670,318 @@
       <c r="E16" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="12" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="13">
         <v>2</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="12">
         <v>1206</v>
       </c>
       <c r="D17" s="10">
         <v>2</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="11">
         <v>2</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="13">
         <v>100</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="12">
         <v>1206</v>
       </c>
       <c r="D18" s="10">
         <v>11</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="11">
         <v>100</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="12" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="13">
         <v>1000</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="12" t="s">
         <v>156</v>
       </c>
       <c r="D19" s="10">
         <v>2</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="11">
         <v>1000</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="12" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="13">
         <v>5000</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>156</v>
       </c>
       <c r="D20" s="10">
         <v>14</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="11">
         <v>4990</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="12" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="13">
         <v>10000</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="12" t="s">
         <v>156</v>
       </c>
       <c r="D21" s="10">
         <v>8</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="11">
         <v>10000</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="12" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="13">
         <v>20000</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="12" t="s">
         <v>156</v>
       </c>
       <c r="D22" s="10">
         <v>1</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="11">
         <v>20000</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="12" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="13">
         <v>200000</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>157</v>
       </c>
       <c r="D23" s="10">
         <v>20</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="11">
         <v>200000</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="12" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D24" s="10">
         <v>2</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="12" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>36</v>
       </c>
       <c r="D25" s="10">
         <v>1</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="12" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>168</v>
       </c>
       <c r="D26" s="10">
         <v>2</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="12" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D27" s="10">
         <v>2</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="12">
         <v>524</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D28" s="10">
         <v>1</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="12" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="12" t="s">
         <v>161</v>
       </c>
       <c r="D29" s="10">
         <v>4</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="12" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="12" t="s">
         <v>167</v>
       </c>
       <c r="D30" s="10">
         <v>1</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="12" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="12" t="s">
         <v>160</v>
       </c>
       <c r="D31" s="10">
         <v>5</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="12" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="13">
         <v>20000</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="12" t="s">
         <v>175</v>
       </c>
       <c r="D32" s="10">
         <v>7</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="12" t="s">
         <v>206</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed OPA77 to AD620
</commit_message>
<xml_diff>
--- a/DOCS/Part list.xlsx
+++ b/DOCS/Part list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{98B7D553-DBA5-4045-B3A1-9F527CC213F4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B44392-D678-46F9-8652-1FB9BF68D48A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Used" sheetId="1" r:id="rId1"/>
@@ -698,7 +698,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -768,7 +768,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
@@ -782,10 +782,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1133,17 +1133,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.73046875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.73046875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.73046875" style="1"/>
+    <col min="1" max="2" width="18.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>31.363200000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1203,21 +1203,21 @@
         <v>6</v>
       </c>
       <c r="D3" s="4">
-        <v>0.61699999999999999</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="E3" s="4">
         <f>D3*1.21</f>
-        <v>0.74656999999999996</v>
+        <v>0.96194999999999997</v>
       </c>
       <c r="F3" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="5">
         <f>F3*E3</f>
-        <v>2.9862799999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+        <v>4.8097500000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>146</v>
       </c>
@@ -1242,14 +1242,14 @@
         <v>3.0975999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>148</v>
       </c>
@@ -1274,14 +1274,14 @@
         <v>17.829999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>27</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>15.9236</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="25"/>
       <c r="C9" s="2" t="s">
@@ -1327,7 +1327,7 @@
         <v>19.432599999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>143</v>
       </c>
@@ -1368,13 +1368,13 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
@@ -1530,10 +1530,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
@@ -1547,11 +1547,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
   </sheetData>
@@ -1603,13 +1603,13 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.73046875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="14.265625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.73046875" style="1"/>
+    <col min="1" max="14" width="14.28515625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>42</v>
       </c>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="N1" s="24"/>
     </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>64</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>136</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
         <v>75</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
         <v>76</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
         <v>77</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E12" s="7" t="s">
         <v>11</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
         <v>89</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
         <v>91</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
         <v>95</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
         <v>96</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>97</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>98</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>99</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="1" t="s">
         <v>101</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
         <v>102</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E22" s="1" t="s">
         <v>103</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E23" s="1" t="s">
         <v>107</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E24" s="1" t="s">
         <v>108</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E25" s="1" t="s">
         <v>110</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" s="1" t="s">
         <v>111</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" s="1" t="s">
         <v>112</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="1" t="s">
         <v>113</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="1" t="s">
         <v>114</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E30" s="1" t="s">
         <v>115</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E31" s="1" t="s">
         <v>116</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="5:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="s">
         <v>117</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="7" t="s">
         <v>119</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="1" t="s">
         <v>120</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="s">
         <v>121</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36" s="1" t="s">
         <v>122</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E37" s="1" t="s">
         <v>125</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="1" t="s">
         <v>126</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E39" s="1" t="s">
         <v>130</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E40" s="1" t="s">
         <v>137</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E41" s="1" t="s">
         <v>138</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E42" s="1" t="s">
         <v>106</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="5:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E43" s="1" t="s">
         <v>105</v>
       </c>
@@ -2344,23 +2344,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D077170-5C74-45B1-BD2D-CC2883FCAE3A}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.59765625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.59765625" style="10"/>
-    <col min="2" max="2" width="9.59765625" style="11"/>
-    <col min="3" max="3" width="9.59765625" style="12"/>
-    <col min="4" max="5" width="9.59765625" style="10"/>
-    <col min="6" max="7" width="9.59765625" style="12"/>
-    <col min="8" max="8" width="18.59765625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="27.59765625" style="10" customWidth="1"/>
-    <col min="10" max="16384" width="9.59765625" style="10"/>
+    <col min="1" max="1" width="9.5703125" style="10"/>
+    <col min="2" max="2" width="9.5703125" style="11"/>
+    <col min="3" max="3" width="9.5703125" style="12"/>
+    <col min="4" max="5" width="9.5703125" style="10"/>
+    <col min="6" max="7" width="9.5703125" style="12"/>
+    <col min="8" max="8" width="18.5703125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="9.5703125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>152</v>
       </c>
@@ -2376,7 +2376,7 @@
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="11" t="s">
         <v>153</v>
@@ -2400,7 +2400,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>155</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>155</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>155</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>155</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>155</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>155</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>155</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>155</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>155</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>164</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>164</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>163</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>169</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>169</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>151</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>151</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>151</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>151</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>151</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>151</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>151</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>158</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>158</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>158</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>158</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>158</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>158</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>158</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>158</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>162</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>164</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="19" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Finalizing components & placement
</commit_message>
<xml_diff>
--- a/DOCS/Part list.xlsx
+++ b/DOCS/Part list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D767E32C-7C03-4718-AF9D-24A273C3A969}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C18907B-D03D-4C68-BCD7-B035ED811DEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="176">
   <si>
     <t>Part</t>
   </si>
@@ -389,15 +389,9 @@
     <t>Capacitors</t>
   </si>
   <si>
-    <t>6032T</t>
-  </si>
-  <si>
     <t>THT</t>
   </si>
   <si>
-    <t>3216T</t>
-  </si>
-  <si>
     <t>RC snubber</t>
   </si>
   <si>
@@ -530,19 +524,61 @@
     <t>lv.farnell.com/coilcraft/mss1260-104mld/inductor-pwr-100uh-2-1a-20-8mhz/dp/2288438</t>
   </si>
   <si>
-    <t>4/7.6 pitch</t>
+    <t>2/7.62 pitch</t>
+  </si>
+  <si>
+    <t>digikey</t>
+  </si>
+  <si>
+    <t>digikey.lv/product-detail/en/amphenol-anytek/T70243500000G/609-3954-ND/2261340</t>
+  </si>
+  <si>
+    <t>Price per</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>lv.farnell.com/ixys-semiconductor/ixtk102n65x2/mosfet-n-ch-650v-102a-to-264p/dp/2674784</t>
+  </si>
+  <si>
+    <t>digikey.lv/products/en?keywords=RFMM-0505S</t>
+  </si>
+  <si>
+    <t>TANT-C</t>
+  </si>
+  <si>
+    <t>5V-&gt;5V coupling</t>
+  </si>
+  <si>
+    <t>TANT-D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -572,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -592,17 +628,29 @@
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="48" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -884,32 +932,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C19687D-3BFF-4D51-B0EC-0CF77A940B00}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="6" customWidth="1"/>
     <col min="2" max="3" width="12.7109375" style="4" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" style="4"/>
+    <col min="4" max="4" width="12.7109375" style="4"/>
+    <col min="5" max="5" width="12.7109375" style="11"/>
     <col min="6" max="6" width="27.7109375" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="12.7109375" style="4"/>
+    <col min="7" max="8" width="12.7109375" style="12"/>
+    <col min="9" max="16384" width="12.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>111</v>
       </c>
@@ -922,811 +974,1026 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="11" t="s">
         <v>117</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="B3" s="4">
+        <v>6332</v>
+      </c>
+      <c r="C3" s="4">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12">
+        <f t="shared" ref="H3:H12" si="0">C3*G3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
         <v>3216</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="B4" s="4">
-        <v>6332</v>
       </c>
       <c r="C4" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4">
-        <v>3216</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="C5" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>121</v>
+        <v>100</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1608</v>
       </c>
       <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H6" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="B7" s="4">
-        <v>2012</v>
+        <v>1608</v>
       </c>
       <c r="C7" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="H7" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>350</v>
+        <v>1000</v>
       </c>
       <c r="B8" s="4">
         <v>1608</v>
       </c>
       <c r="C8" s="4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>1000</v>
+        <v>2150</v>
       </c>
       <c r="B9" s="4">
+        <v>2012</v>
+      </c>
+      <c r="C9" s="4">
+        <v>10</v>
+      </c>
+      <c r="H9" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>10000</v>
+      </c>
+      <c r="B10" s="4">
         <v>1608</v>
       </c>
-      <c r="C9" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>2150</v>
-      </c>
-      <c r="B10" s="4">
-        <v>2012</v>
-      </c>
       <c r="C10" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H10" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="B11" s="4">
         <v>1608</v>
       </c>
       <c r="C11" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H11" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>100000</v>
+        <v>2000000</v>
       </c>
       <c r="B12" s="4">
+        <v>3216</v>
+      </c>
+      <c r="C12" s="4">
+        <v>5</v>
+      </c>
+      <c r="H12" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>1.5E-11</v>
+      </c>
+      <c r="B16" s="4">
         <v>1608</v>
       </c>
-      <c r="C12" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>2000000</v>
-      </c>
-      <c r="B13" s="4">
-        <v>3216</v>
-      </c>
-      <c r="C13" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="4">
+        <v>14</v>
+      </c>
+      <c r="H16" s="12">
+        <f>C16*G16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
-        <v>1.5E-11</v>
+        <v>4.7000000000000003E-10</v>
       </c>
       <c r="B17" s="4">
         <v>1608</v>
       </c>
       <c r="C17" s="4">
+        <v>5</v>
+      </c>
+      <c r="H17" s="12">
+        <f t="shared" ref="H17:H26" si="1">C17*G17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="5" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>1E-8</v>
+      </c>
+      <c r="B19" s="4">
+        <v>2012</v>
+      </c>
+      <c r="C19" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>1E-10</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="H19" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="B20" s="4">
         <v>1608</v>
       </c>
-      <c r="C18" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>5.0000000000000003E-10</v>
-      </c>
-      <c r="B19" s="4">
+      <c r="C20" s="4">
+        <v>37</v>
+      </c>
+      <c r="H20" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>1.4999999999999999E-7</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>4.7E-7</v>
+      </c>
+      <c r="B22" s="4">
         <v>1608</v>
       </c>
-      <c r="C19" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>1E-8</v>
-      </c>
-      <c r="B20" s="4">
-        <v>2012</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
+      <c r="H22" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>4.6999999999999999E-6</v>
+      </c>
+      <c r="B23" s="4">
+        <v>3216</v>
+      </c>
+      <c r="C23" s="4">
+        <v>8</v>
+      </c>
+      <c r="H23" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>1E-8</v>
-      </c>
-      <c r="B21" s="4">
-        <v>3216</v>
-      </c>
-      <c r="C21" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>1E-8</v>
-      </c>
-      <c r="B22" s="4">
-        <v>2012</v>
-      </c>
-      <c r="C22" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>9.9999999999999995E-8</v>
-      </c>
-      <c r="B23" s="4">
-        <v>1608</v>
-      </c>
-      <c r="C23" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>9.9999999999999995E-8</v>
-      </c>
-      <c r="B24" s="4">
-        <v>3216</v>
-      </c>
-      <c r="C24" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
-        <v>1.4999999999999999E-7</v>
+        <v>4.6999999999999997E-5</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>121</v>
+        <v>175</v>
       </c>
       <c r="C25" s="4">
         <v>1</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="H25" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>2.2000000000000001E-4</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="4">
+        <v>3</v>
+      </c>
+      <c r="H26" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="4">
+        <v>2</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H30" s="12">
+        <f>C30*G30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="4">
+        <v>5</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H31" s="12">
+        <f t="shared" ref="H31:H38" si="2">C31*G31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="4">
+        <v>7</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H32" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>3.3000000000000002E-7</v>
-      </c>
-      <c r="B26" s="4">
-        <v>3216</v>
-      </c>
-      <c r="C26" s="4">
+      <c r="B33" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="B27" s="4">
-        <v>3216</v>
-      </c>
-      <c r="C27" s="4">
+      <c r="D33" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H33" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="4">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>4.6999999999999999E-6</v>
-      </c>
-      <c r="B29" s="4">
-        <v>3216</v>
-      </c>
-      <c r="C29" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C30" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>2.1999999999999999E-5</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C31" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
-        <v>2.2000000000000001E-4</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C32" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="D35" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="H35" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C36" s="4">
         <v>2</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="H36" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C37" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="H37" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>33</v>
+        <v>132</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="C38" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" s="4">
+        <v>141</v>
+      </c>
+      <c r="H38" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" s="4">
-        <v>2</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C42" s="4">
         <v>2</v>
       </c>
       <c r="D42" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H42" s="12">
+        <f>C42*G42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>133</v>
-      </c>
       <c r="B43" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C43" s="4">
         <v>4</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F43" s="4" t="s">
+      <c r="H43" s="12">
+        <f t="shared" ref="H43:H47" si="3">C43*G43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="4">
+        <v>16</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" s="4">
+      <c r="H44" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="4">
+        <v>4</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H45" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="4">
+        <v>2</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="G46" s="12">
+        <v>12.88</v>
+      </c>
+      <c r="H46" s="12">
+        <f t="shared" si="3"/>
+        <v>25.76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="4">
+        <v>4</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H47" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+    </row>
+    <row r="50" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-    </row>
-    <row r="47" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="4" t="s">
+      <c r="E50" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="4">
         <v>1</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C48" s="4">
-        <v>2</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C49" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C50" s="4">
-        <v>16</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" s="4">
-        <v>4</v>
-      </c>
       <c r="D51" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="H51" s="12">
+        <f t="shared" ref="H51:H53" si="4">G51*C51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>3</v>
+        <v>152</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C52" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="C53" s="4">
+        <v>1</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H53" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" s="4">
+        <v>2</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G54" s="12">
+        <v>0.89</v>
+      </c>
+      <c r="H54" s="12">
+        <f>G54*C54</f>
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+    </row>
+    <row r="57" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="8">
+        <v>2</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+      <c r="E58" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F58" s="3"/>
+      <c r="G58" s="12">
+        <v>1.22</v>
+      </c>
+      <c r="H58" s="12">
+        <f>G58*C58</f>
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C59" s="4">
+        <v>2</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-    </row>
-    <row r="56" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="4" t="s">
+      <c r="H59" s="12">
+        <f t="shared" ref="H59:H62" si="5">G59*C59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C60" s="4">
+        <v>4</v>
+      </c>
+      <c r="H60" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" s="4">
         <v>1</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C57" s="4">
-        <v>1</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C58" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C59" s="4">
-        <v>1</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="C60" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-    </row>
-    <row r="63" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="9">
-        <v>2</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E64" s="10" t="s">
+      <c r="D61" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C65" s="4">
-        <v>2</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C66" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="E61" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F61" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="G61" s="12">
+        <v>1.45</v>
+      </c>
+      <c r="H61" s="12">
+        <f t="shared" si="5"/>
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C67" s="4">
-        <v>1</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
-        <v>164</v>
+      <c r="H62" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" s="13"/>
+      <c r="C64" s="8">
+        <f>SUM(C58:C63,C51:C55,C42:C48,C30:C39,C16:C27,C3:C13)</f>
+        <v>260</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="12">
+        <f>SUM(H58:H63,H51:H55,H42:H48,H30:H39,H16:H27,H3:H13)</f>
+        <v>31.43</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A36:F44">
-    <sortCondition ref="A36:A44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A30:F38">
+    <sortCondition ref="A30:A38"/>
   </sortState>
-  <mergeCells count="6">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A62:F62"/>
+  <mergeCells count="7">
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A56:H56"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1745,34 +2012,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5" t="s">
+      <c r="L1" s="9"/>
+      <c r="M1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="5"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>